<commit_message>
Updated Comments to the USA Model and Ran the Commented Version
</commit_message>
<xml_diff>
--- a/SDG USA Model/usaoutput.xlsx
+++ b/SDG USA Model/usaoutput.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\gamsdir\projdir\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Wi2050\SDG USA Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6F0643E-B0F7-413B-9896-7AFA9A728220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E67D2D8-EF3E-40E9-BDF3-C42A119A7148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="368" yWindow="368" windowWidth="11272" windowHeight="7492" activeTab="2" xr2:uid="{ADCA1185-D635-4A1C-9878-2479910602B2}"/>
+    <workbookView xWindow="31200" yWindow="2400" windowWidth="21600" windowHeight="11235" activeTab="2" xr2:uid="{ADCA1185-D635-4A1C-9878-2479910602B2}"/>
   </bookViews>
   <sheets>
     <sheet name="qpcs" sheetId="1" r:id="rId1"/>
     <sheet name="poptots" sheetId="2" r:id="rId2"/>
     <sheet name="tfrs" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,9 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -485,9 +483,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -576,7 +574,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -668,96 +666,96 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>52.637324622658795</v>
+        <v>3.3160863265614821E-2</v>
       </c>
       <c r="C3">
-        <v>60.799263548951757</v>
+        <v>7.2055679344342413E-3</v>
       </c>
       <c r="D3">
-        <v>60.035879035896123</v>
+        <v>24.783628828465101</v>
       </c>
       <c r="E3">
-        <v>59.840559912414427</v>
+        <v>24.436723759512404</v>
       </c>
       <c r="F3">
-        <v>61.120059726484918</v>
+        <v>23.853123346199133</v>
       </c>
       <c r="G3">
-        <v>60.553945600496469</v>
+        <v>22.87618944730465</v>
       </c>
       <c r="H3">
-        <v>60.480117229990618</v>
+        <v>22.0691588666553</v>
       </c>
       <c r="I3">
-        <v>60.374480812743265</v>
+        <v>21.278982930462952</v>
       </c>
       <c r="J3">
-        <v>61.053733565664572</v>
+        <v>20.503518574885792</v>
       </c>
       <c r="K3">
-        <v>61.658518543095141</v>
+        <v>19.495660854534947</v>
       </c>
       <c r="L3">
-        <v>60.711641724357939</v>
+        <v>18.524304406094032</v>
       </c>
       <c r="M3">
-        <v>60.469376647916469</v>
+        <v>17.587934371124174</v>
       </c>
       <c r="N3">
-        <v>60.903279817344085</v>
+        <v>16.79856625473678</v>
       </c>
       <c r="O3">
-        <v>60.555016030190266</v>
+        <v>16.037446820516152</v>
       </c>
       <c r="P3">
-        <v>58.75811982232873</v>
+        <v>15.420539193297174</v>
       </c>
       <c r="Q3">
-        <v>58.458589764487719</v>
+        <v>14.833148740858993</v>
       </c>
       <c r="R3">
-        <v>58.869401970810394</v>
+        <v>14.275633082908154</v>
       </c>
       <c r="S3">
-        <v>59.288578463528495</v>
+        <v>13.64478348384297</v>
       </c>
       <c r="T3">
-        <v>57.628131167040991</v>
+        <v>13.04519922477783</v>
       </c>
       <c r="U3">
-        <v>56.736645524799826</v>
+        <v>12.477607357163503</v>
       </c>
       <c r="V3">
-        <v>56.576956040448103</v>
+        <v>11.94071347255176</v>
       </c>
       <c r="W3">
-        <v>56.446625320370948</v>
+        <v>11.431774727993492</v>
       </c>
       <c r="X3">
-        <v>54.984582371492301</v>
+        <v>10.940457653168236</v>
       </c>
       <c r="Y3">
-        <v>54.856111720500088</v>
+        <v>10.47235787881006</v>
       </c>
       <c r="Z3">
-        <v>53.79853445006578</v>
+        <v>9.8862694696671269</v>
       </c>
       <c r="AA3">
-        <v>51.807787376210669</v>
+        <v>9.3136669486947845</v>
       </c>
       <c r="AB3">
-        <v>50.763309929274257</v>
+        <v>8.7515743393907748</v>
       </c>
       <c r="AC3">
-        <v>48.785172736262368</v>
+        <v>8.3835131349724126</v>
       </c>
       <c r="AD3">
-        <v>48.188295945005635</v>
+        <v>8.0175294140449829</v>
       </c>
     </row>
   </sheetData>
@@ -771,9 +769,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -862,7 +860,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -873,88 +871,88 @@
         <v>329.41237467204257</v>
       </c>
       <c r="D2">
-        <v>327.96023036697682</v>
+        <v>327.9607291585225</v>
       </c>
       <c r="E2">
-        <v>326.47780372544861</v>
+        <v>326.47850816312393</v>
       </c>
       <c r="F2">
-        <v>324.94692766673535</v>
+        <v>324.94748738725059</v>
       </c>
       <c r="G2">
-        <v>323.35135697597184</v>
+        <v>323.35191721027951</v>
       </c>
       <c r="H2">
-        <v>321.6968174382456</v>
+        <v>321.69712123146473</v>
       </c>
       <c r="I2">
-        <v>319.97386988094996</v>
+        <v>319.97440748669231</v>
       </c>
       <c r="J2">
-        <v>318.18279392838963</v>
+        <v>318.1838636852242</v>
       </c>
       <c r="K2">
-        <v>316.3223364574182</v>
+        <v>316.32340330668472</v>
       </c>
       <c r="L2">
-        <v>314.38881093911868</v>
+        <v>314.38989408033956</v>
       </c>
       <c r="M2">
-        <v>312.38061231609919</v>
+        <v>312.38169507430638</v>
       </c>
       <c r="N2">
-        <v>310.28977310095235</v>
+        <v>310.29085564087842</v>
       </c>
       <c r="O2">
-        <v>308.11419400921778</v>
+        <v>308.11527653084659</v>
       </c>
       <c r="P2">
-        <v>305.85263606881256</v>
+        <v>305.85380269945551</v>
       </c>
       <c r="Q2">
-        <v>303.49878617126365</v>
+        <v>303.49999287686194</v>
       </c>
       <c r="R2">
-        <v>301.05268113930174</v>
+        <v>301.0542481795386</v>
       </c>
       <c r="S2">
-        <v>298.50967617548042</v>
+        <v>298.51097141646994</v>
       </c>
       <c r="T2">
-        <v>295.86762650627384</v>
+        <v>295.86892288053224</v>
       </c>
       <c r="U2">
-        <v>293.12614087043869</v>
+        <v>293.12743706669545</v>
       </c>
       <c r="V2">
-        <v>290.28161172196099</v>
+        <v>290.28277589431121</v>
       </c>
       <c r="W2">
-        <v>287.33544473314095</v>
+        <v>287.33722947333507</v>
       </c>
       <c r="X2">
-        <v>284.28780394853396</v>
+        <v>284.28958506804616</v>
       </c>
       <c r="Y2">
-        <v>281.14026602137199</v>
+        <v>281.14244513064693</v>
       </c>
       <c r="Z2">
-        <v>277.89422364398706</v>
+        <v>277.89639914115367</v>
       </c>
       <c r="AA2">
-        <v>274.54887504628715</v>
+        <v>274.55104931746502</v>
       </c>
       <c r="AB2">
-        <v>271.11058024957839</v>
+        <v>271.11275401390276</v>
       </c>
       <c r="AC2">
-        <v>267.58326297441528</v>
+        <v>267.58543615617805</v>
       </c>
       <c r="AD2">
-        <v>263.97160904811199</v>
+        <v>263.97378162914174</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -965,85 +963,85 @@
         <v>329.41237467204257</v>
       </c>
       <c r="D3">
-        <v>331.88051723955141</v>
+        <v>331.91762326643249</v>
       </c>
       <c r="E3">
-        <v>334.40118195375044</v>
+        <v>334.54555394105523</v>
       </c>
       <c r="F3">
-        <v>337.00233328470398</v>
+        <v>337.33603708817583</v>
       </c>
       <c r="G3">
-        <v>339.67445103739703</v>
+        <v>340.25269948509094</v>
       </c>
       <c r="H3">
-        <v>342.39925275624034</v>
+        <v>343.25201467364519</v>
       </c>
       <c r="I3">
-        <v>345.21702166471607</v>
+        <v>346.33127850705199</v>
       </c>
       <c r="J3">
-        <v>348.10316836951608</v>
+        <v>349.49258843492021</v>
       </c>
       <c r="K3">
-        <v>350.99580867524924</v>
+        <v>352.69991389817426</v>
       </c>
       <c r="L3">
-        <v>353.8895620931645</v>
+        <v>355.9209350839684</v>
       </c>
       <c r="M3">
-        <v>356.79930331095375</v>
+        <v>359.15542988531359</v>
       </c>
       <c r="N3">
-        <v>359.78498456170166</v>
+        <v>362.37122544898722</v>
       </c>
       <c r="O3">
-        <v>362.7569816519341</v>
+        <v>365.5842723085118</v>
       </c>
       <c r="P3">
-        <v>365.59651912064356</v>
+        <v>368.67521120609308</v>
       </c>
       <c r="Q3">
-        <v>368.2599378797633</v>
+        <v>371.64051068963164</v>
       </c>
       <c r="R3">
-        <v>370.8171152620435</v>
+        <v>374.46124701230633</v>
       </c>
       <c r="S3">
-        <v>373.28919136072074</v>
+        <v>377.14925518505817</v>
       </c>
       <c r="T3">
-        <v>375.60712348735512</v>
+        <v>379.66042940928611</v>
       </c>
       <c r="U3">
-        <v>377.61723178510562</v>
+        <v>381.90514947017459</v>
       </c>
       <c r="V3">
-        <v>379.38142431073612</v>
+        <v>383.88199945058159</v>
       </c>
       <c r="W3">
-        <v>380.88029742574645</v>
+        <v>385.57638340781511</v>
       </c>
       <c r="X3">
-        <v>382.14810245682099</v>
+        <v>386.98179264667539</v>
       </c>
       <c r="Y3">
-        <v>383.14479482987451</v>
+        <v>388.10006480221875</v>
       </c>
       <c r="Z3">
-        <v>383.99448598437374</v>
+        <v>389.00679065960821</v>
       </c>
       <c r="AA3">
-        <v>384.64809460518546</v>
+        <v>389.70681486805688</v>
       </c>
       <c r="AB3">
-        <v>385.10737410020198</v>
+        <v>390.21329542916254</v>
       </c>
       <c r="AC3">
-        <v>385.37001708022592</v>
+        <v>390.49946876967931</v>
       </c>
       <c r="AD3">
-        <v>385.46610923219117</v>
+        <v>390.61386697999529</v>
       </c>
     </row>
   </sheetData>
@@ -1057,9 +1055,9 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1148,7 +1146,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1162,85 +1160,85 @@
         <v>1.7386310920766965</v>
       </c>
       <c r="E2">
-        <v>1.7326434975161813</v>
+        <v>1.736810445935659</v>
       </c>
       <c r="F2">
-        <v>1.7394679370437816</v>
+        <v>1.7434032361965357</v>
       </c>
       <c r="G2">
-        <v>1.7463106835848445</v>
+        <v>1.7501665732723115</v>
       </c>
       <c r="H2">
-        <v>1.7533849465723537</v>
+        <v>1.7571223846202748</v>
       </c>
       <c r="I2">
-        <v>1.7596382371633594</v>
+        <v>1.7632894886286188</v>
       </c>
       <c r="J2">
-        <v>1.7658965055973246</v>
+        <v>1.7695010124491959</v>
       </c>
       <c r="K2">
-        <v>1.7721761209424371</v>
+        <v>1.7759093674728277</v>
       </c>
       <c r="L2">
-        <v>1.7784556472049513</v>
+        <v>1.7823169779637831</v>
       </c>
       <c r="M2">
-        <v>1.7850058156297617</v>
+        <v>1.7892228912239156</v>
       </c>
       <c r="N2">
-        <v>1.7869913580598105</v>
+        <v>1.7920777941962298</v>
       </c>
       <c r="O2">
-        <v>1.8016016695984838</v>
+        <v>1.8016016695984836</v>
       </c>
       <c r="P2">
-        <v>1.803482664659019</v>
+        <v>1.8034826646590187</v>
       </c>
       <c r="Q2">
-        <v>1.8053636597195541</v>
+        <v>1.8053636597195539</v>
       </c>
       <c r="R2">
-        <v>1.7978273887874856</v>
+        <v>1.8011350515831483</v>
       </c>
       <c r="S2">
-        <v>1.7815525407499442</v>
+        <v>1.786242003059368</v>
       </c>
       <c r="T2">
-        <v>1.766201196781475</v>
+        <v>1.7699398093001781</v>
       </c>
       <c r="U2">
-        <v>1.7498990015850577</v>
+        <v>1.7536376141037608</v>
       </c>
       <c r="V2">
-        <v>1.7352959295601407</v>
+        <v>1.7373354189073436</v>
       </c>
       <c r="W2">
-        <v>1.6869753685275237</v>
+        <v>1.7021101136094534</v>
       </c>
       <c r="X2">
-        <v>1.6293513314101378</v>
+        <v>1.6528490961154654</v>
       </c>
       <c r="Y2">
-        <v>1.5713818097876191</v>
+        <v>1.5915581929550278</v>
       </c>
       <c r="Z2">
-        <v>1.5137509687210111</v>
+        <v>1.5340366849660163</v>
       </c>
       <c r="AA2">
-        <v>1.4583952102445965</v>
+        <v>1.4727457762823399</v>
       </c>
       <c r="AB2">
-        <v>1.3708078921938427</v>
+        <v>1.4006361306687767</v>
       </c>
       <c r="AC2">
-        <v>1.2824077757392707</v>
+        <v>1.3288052108154684</v>
       </c>
       <c r="AD2">
-        <v>1.1873787788021568</v>
+        <v>1.2314324917060495</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1248,88 +1246,88 @@
         <v>1.7315820947944578</v>
       </c>
       <c r="C3">
-        <v>1.7316442921798232</v>
+        <v>1.7315651724807068</v>
       </c>
       <c r="D3">
-        <v>1.736598130763352</v>
+        <v>1.7354175299663821</v>
       </c>
       <c r="E3">
-        <v>1.7410589622702501</v>
+        <v>1.7386826290225417</v>
       </c>
       <c r="F3">
-        <v>1.7455197937771485</v>
+        <v>1.7422071276636613</v>
       </c>
       <c r="G3">
-        <v>1.7488864910153969</v>
+        <v>1.7490594240720367</v>
       </c>
       <c r="H3">
-        <v>1.7523880449344693</v>
+        <v>1.7561481753433255</v>
       </c>
       <c r="I3">
-        <v>1.7550590230234295</v>
+        <v>1.7627517140379605</v>
       </c>
       <c r="J3">
-        <v>1.7533721754744664</v>
+        <v>1.7694280346190929</v>
       </c>
       <c r="K3">
-        <v>1.7516853979080029</v>
+        <v>1.7761043552002285</v>
       </c>
       <c r="L3">
-        <v>1.7505169725854666</v>
+        <v>1.7823682450912059</v>
       </c>
       <c r="M3">
-        <v>1.7569150398469564</v>
+        <v>1.7888756324315942</v>
       </c>
       <c r="N3">
-        <v>1.7539427934067746</v>
+        <v>1.7926616125485402</v>
       </c>
       <c r="O3">
-        <v>1.7517908254368011</v>
+        <v>1.7968558037490023</v>
       </c>
       <c r="P3">
-        <v>1.7501606919994912</v>
+        <v>1.8010499949494645</v>
       </c>
       <c r="Q3">
-        <v>1.7551757172418092</v>
+        <v>1.8029309900099999</v>
       </c>
       <c r="R3">
-        <v>1.758760855214982</v>
+        <v>1.804724850884714</v>
       </c>
       <c r="S3">
-        <v>1.7537245535708812</v>
+        <v>1.8037215414764098</v>
       </c>
       <c r="T3">
-        <v>1.7519407340396496</v>
+        <v>1.8031378076105611</v>
       </c>
       <c r="U3">
-        <v>1.7562873069896119</v>
+        <v>1.8025540737447088</v>
       </c>
       <c r="V3">
-        <v>1.7536753024428346</v>
+        <v>1.799592745138284</v>
       </c>
       <c r="W3">
-        <v>1.7530329971459477</v>
+        <v>1.7965765730397862</v>
       </c>
       <c r="X3">
-        <v>1.7588233006044973</v>
+        <v>1.7945407916589886</v>
       </c>
       <c r="Y3">
-        <v>1.7668380728714128</v>
+        <v>1.7923579516705104</v>
       </c>
       <c r="Z3">
-        <v>1.7740321165127462</v>
+        <v>1.7901751116820606</v>
       </c>
       <c r="AA3">
-        <v>1.7774265449644344</v>
+        <v>1.7888256038036161</v>
       </c>
       <c r="AB3">
-        <v>1.7752278286376064</v>
+        <v>1.7874602195868192</v>
       </c>
       <c r="AC3">
-        <v>1.783028755183022</v>
+        <v>1.786717694516426</v>
       </c>
       <c r="AD3">
-        <v>1.789903694022857</v>
+        <v>1.7858817405740814</v>
       </c>
     </row>
   </sheetData>

</xml_diff>